<commit_message>
sk 2021/7/20 sheet1 A4セルに"git練習用4"を追加
</commit_message>
<xml_diff>
--- a/練習用ファイル.xlsx
+++ b/練習用ファイル.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Git練習用</t>
     <rPh sb="3" eb="6">
@@ -41,6 +41,13 @@
   </si>
   <si>
     <t>Git練習用3</t>
+    <rPh sb="3" eb="6">
+      <t>レンシュウヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Git練習用4</t>
     <rPh sb="3" eb="6">
       <t>レンシュウヨウ</t>
     </rPh>
@@ -374,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -397,6 +404,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sk 20210720 git diff確認
</commit_message>
<xml_diff>
--- a/練習用ファイル.xlsx
+++ b/練習用ファイル.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Git練習用</t>
     <rPh sb="3" eb="6">
@@ -82,6 +82,16 @@
   </si>
   <si>
     <t>Git練習用7</t>
+    <rPh sb="3" eb="5">
+      <t>レンシュウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Git練習用8</t>
     <rPh sb="3" eb="5">
       <t>レンシュウ</t>
     </rPh>
@@ -418,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -449,6 +459,11 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>